<commit_message>
update consolidated extraction data
</commit_message>
<xml_diff>
--- a/data/extraction_merged.xlsx
+++ b/data/extraction_merged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4FAF05A-501D-4E9A-9CB7-A66F7EC0B821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6A4D40F1-1687-46DD-80EF-C16CAA468707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="289" uniqueCount="91">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="293" uniqueCount="90">
   <si>
     <t>Title</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>The OMiLAB Digital Innovation environment: Agile conceptual models to bridge business value with Digital and Physical Twins for Product-Service Systems development</t>
-  </si>
-  <si>
-    <t>Not Available</t>
   </si>
   <si>
     <t>Digital twin enhanced human-machine interaction in product lifecycle</t>
@@ -319,7 +316,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,19 +453,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -656,19 +646,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,18 +817,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1202,8 +1184,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,26 +1214,26 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="2" t="str">
         <f>E2</f>
         <v>OK</v>
@@ -1261,17 +1243,17 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3"/>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G62" si="0">E3</f>
         <v>Challenge/Position Paper</v>
@@ -1281,17 +1263,17 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1341,17 +1323,17 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3"/>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1361,17 +1343,17 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1381,17 +1363,17 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3"/>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1421,17 +1403,17 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3"/>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1441,17 +1423,17 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1501,17 +1483,17 @@
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1541,36 +1523,36 @@
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" t="str">
         <f>D17</f>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="2" t="str">
+      <c r="B18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="str">
         <f t="shared" ref="G18:G28" si="1">D18</f>
         <v>OK</v>
       </c>
@@ -1579,36 +1561,36 @@
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="2" t="str">
+      <c r="B20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
@@ -1617,15 +1599,15 @@
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
         <v>No MDE technique used</v>
@@ -1635,15 +1617,15 @@
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
         <v>Challenge/Position Paper</v>
@@ -1653,15 +1635,15 @@
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
         <v>Challenge/Position Paper</v>
@@ -1671,36 +1653,36 @@
       <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" t="str">
+      <c r="B25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
@@ -1709,15 +1691,15 @@
       <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
         <v>No MDE technique used</v>
@@ -1727,15 +1709,17 @@
       <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
         <v>No MDE technique used</v>
@@ -1745,15 +1729,17 @@
       <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -1772,6 +1758,8 @@
       <c r="D29" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
       <c r="G29" t="str">
         <f>D29</f>
         <v>No Model used</v>
@@ -1790,6 +1778,8 @@
       <c r="D30" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
       <c r="G30" t="str">
         <f>D30</f>
         <v>No Model used</v>
@@ -1808,6 +1798,8 @@
       <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
       <c r="G31" t="str">
         <f>D31</f>
         <v>No MDE technique used</v>
@@ -1817,17 +1809,17 @@
       <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="5"/>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="3"/>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1837,15 +1829,15 @@
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="7"/>
+      <c r="B33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3"/>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1855,92 +1847,92 @@
       <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="7"/>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" t="str">
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" t="str">
+      <c r="B36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="4"/>
-      <c r="G38" t="str">
+      <c r="B38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
@@ -1949,15 +1941,15 @@
       <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="6"/>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3"/>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1967,15 +1959,15 @@
       <c r="A40" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="6"/>
+      <c r="B40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3"/>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -1985,15 +1977,15 @@
       <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="6"/>
+      <c r="B41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="3"/>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -2003,15 +1995,15 @@
       <c r="A42" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="6"/>
+      <c r="B42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="3"/>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -2021,63 +2013,63 @@
       <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="6"/>
+      <c r="B43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3"/>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" s="9"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" s="6"/>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="3"/>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -2087,15 +2079,15 @@
       <c r="A47" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="6"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="3"/>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
         <v>No MDE technique used</v>
@@ -2105,16 +2097,17 @@
       <c r="A48" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="5"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="3"/>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2124,16 +2117,17 @@
       <c r="A49" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F49" s="5"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="3"/>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2143,16 +2137,17 @@
       <c r="A50" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="5"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="3"/>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2162,16 +2157,17 @@
       <c r="A51" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="5"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="3"/>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2181,16 +2177,17 @@
       <c r="A52" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="5"/>
+      <c r="F52" s="3"/>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
         <v>No Model used</v>
@@ -2200,107 +2197,118 @@
       <c r="A53" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="7" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
       <c r="G53" t="str">
         <f>D53</f>
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" t="str">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="6" t="str">
         <f t="shared" ref="G54:G55" si="2">D54</f>
-        <v>OK</v>
+        <v>No MDE technique used</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
       <c r="G55" t="str">
         <f t="shared" si="2"/>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="B56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
         <v>6</v>
       </c>
@@ -2318,18 +2326,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="3"/>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2337,18 +2346,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="3"/>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2356,320 +2366,334 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>No MDE technique used</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="5"/>
-      <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="6" t="str">
+        <f t="shared" ref="G63:G70" si="3">D63</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B63" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" t="str">
-        <f>D63</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B64" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B64" t="s">
-        <v>90</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" t="str">
-        <f>D64</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" t="str">
-        <f>D65</f>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="6" t="str">
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
       <c r="G66" t="str">
-        <f>D66</f>
+        <f t="shared" si="3"/>
         <v>No MDE technique used</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
       <c r="G67" t="str">
-        <f>D67</f>
+        <f t="shared" si="3"/>
         <v>No MDE technique used</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
       <c r="G68" t="str">
-        <f>D68</f>
+        <f t="shared" si="3"/>
         <v>No MDE technique used</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" t="str">
+        <f t="shared" si="3"/>
+        <v>No MDE technique used</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" t="str">
-        <f>D69</f>
-        <v>No MDE technique used</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F70" s="4"/>
-      <c r="G70" t="str">
-        <f>D70</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>82</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
       <c r="G72" t="str">
         <f>D72</f>
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" t="s">
-        <v>90</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" t="str">
+    <row r="73" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="6" t="str">
         <f>D73</f>
         <v>OK</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F74" s="6"/>
-      <c r="G74" t="str">
-        <f t="shared" ref="G74:G78" si="3">E74</f>
+    <row r="74" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="7"/>
+      <c r="G74" s="6" t="str">
+        <f t="shared" ref="G74:G78" si="4">E74</f>
         <v>OK</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E75" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F75" s="7"/>
+      <c r="F75" s="3"/>
       <c r="G75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Challenge/Position Paper</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="3"/>
+      <c r="G76" t="str">
+        <f t="shared" si="4"/>
+        <v>Challenge/Position Paper</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="7" t="s">
+      <c r="B77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F76" s="7"/>
-      <c r="G76" t="str">
-        <f t="shared" si="3"/>
-        <v>Challenge/Position Paper</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="E77" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="7"/>
+      <c r="G77" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B77" t="s">
-        <v>90</v>
-      </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="10"/>
-      <c r="G77" t="str">
-        <f t="shared" si="3"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="6" t="str">
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>88</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F78" s="6"/>
-      <c r="G78" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-    </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
update jingxi: 7 papers extracted
</commit_message>
<xml_diff>
--- a/data/extraction_merged.xlsx
+++ b/data/extraction_merged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac130903\Desktop\MDE4DT\mde4dts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5029CDA3-0B5C-4D21-9B0A-EED588AECFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7E72E306-AECF-4A0E-9C40-DFF7CD14B344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction_merged" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -827,48 +825,48 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -884,7 +882,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1184,10 +1182,10 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:C15"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="141.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
@@ -1869,7 +1867,7 @@
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>6</v>
@@ -1889,7 +1887,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>6</v>
@@ -1925,7 +1923,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>6</v>
@@ -2543,7 +2541,7 @@
         <v>6</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>6</v>
@@ -2656,7 +2654,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>6</v>
@@ -2713,7 +2711,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update review intersetions based on jingxi reviews
</commit_message>
<xml_diff>
--- a/data/extraction_merged.xlsx
+++ b/data/extraction_merged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac130903\Desktop\MDE4DT\mde4dts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CCD40C67-93A3-4F5A-837A-65F2D4A90254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2A971449-9298-4CA7-B087-F0899F227E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction_merged" sheetId="1" r:id="rId1"/>
@@ -822,48 +822,48 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -879,7 +879,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1175,22 +1175,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="141.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="141.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1395,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1452,7 +1455,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1698,7 +1701,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
         <v>45</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1969,7 +1972,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4" t="s">
         <v>51</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2056,7 +2059,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>No Model used</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -2571,7 +2574,7 @@
         <v>No MDE technique used</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -2629,7 +2632,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>Challenge/Position Paper</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -2695,7 +2698,23 @@
       <c r="F79" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G78" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G78" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2707,7 +2726,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>